<commit_message>
add a requirement page for SOG.
</commit_message>
<xml_diff>
--- a/smt_refresh_fw_evaluation.xlsx
+++ b/smt_refresh_fw_evaluation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://schneiderelectric-my.sharepoint.com/personal/sesa153954_se_com/Documents/Working/smt_refresh/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\prj\smt_refresh\smt_refresh_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="372" documentId="8_{F4E7F1BA-B40D-4D6F-89BC-5A53FA4C5BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B7DE947-EE5C-40CD-8354-EE619720F36C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752F04F3-FDBE-4AE4-8FE5-0FEBEA55C896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-1500" windowWidth="23256" windowHeight="13896" activeTab="4" xr2:uid="{20390CD0-9F3C-4FAF-AAB0-2CABDDBF005D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{20390CD0-9F3C-4FAF-AAB0-2CABDDBF005D}"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="UPS Protocol" sheetId="3" r:id="rId3"/>
     <sheet name="Event Log" sheetId="4" r:id="rId4"/>
     <sheet name="Firmware Upgrade" sheetId="5" r:id="rId5"/>
+    <sheet name="SOG" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
   <si>
     <t>SMT Refresh Required Features</t>
   </si>
@@ -559,6 +560,40 @@
   </si>
   <si>
     <t>If the Adaptor validates the firmware upgrade image as invalid, Adaptor should reject the firmware installation step.</t>
+  </si>
+  <si>
+    <t>LCD should be able to configure outlet group settings.</t>
+  </si>
+  <si>
+    <t>LCD should be able to control all outlet groups.</t>
+  </si>
+  <si>
+    <t>LCD panel should display outlet group countdown timer if there is a on-going outlet group operation.</t>
+  </si>
+  <si>
+    <t>Required settings:
+1. Turn On Delay
+2. Turn Off Delay
+3. Reboot Duration
+4. Minimum Return Runtime
+5. LoadShed Time On Battery Config
+6. LoadShed Time On Battery Setting
+7. LoadShed Runtime Remain Config
+8. LoadShed Runtime Remain Setting</t>
+  </si>
+  <si>
+    <t>Outlet groups:
+* Main Group Outlets
+* Group Outlets 1</t>
+  </si>
+  <si>
+    <t>Details</t>
+  </si>
+  <si>
+    <t>Fearure - Swithced Outlet Group (SOG)</t>
+  </si>
+  <si>
+    <t>The communication protocol between Adaptor and UPS is switched from the  protocol used under normal conditions to Xmodem with 128 bytes CRC mode.</t>
   </si>
 </sst>
 </file>
@@ -660,7 +695,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -706,11 +741,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1049,7 +1086,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,7 +1291,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,10 +1302,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="16"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -1336,33 +1373,37 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CA4D097-EB0E-4CC4-85E1-D8AEFC1F42DF}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="63.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="74" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="16"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="17"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C2" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1370,7 +1411,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -1378,7 +1419,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>3</v>
       </c>
@@ -1386,7 +1427,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>4</v>
       </c>
@@ -1394,7 +1435,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>5</v>
       </c>
@@ -1402,15 +1443,18 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>6</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="12">
         <v>7</v>
       </c>
@@ -1418,7 +1462,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="12">
         <v>8</v>
       </c>
@@ -1426,7 +1470,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
         <v>9</v>
       </c>
@@ -1434,7 +1478,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>10</v>
       </c>
@@ -1442,6 +1486,86 @@
         <v>51</v>
       </c>
     </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC5EE8D-1107-4292-BA48-0DBC134BF805}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="68.85546875" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="17"/>
+    </row>
+    <row r="2" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>3</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
update the firmware upgrade requirements.
</commit_message>
<xml_diff>
--- a/smt_refresh_fw_evaluation.xlsx
+++ b/smt_refresh_fw_evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\prj\smt_refresh\smt_refresh_plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{199674DA-D7EF-4D05-86D5-923FAEC71651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE29C400-3DAC-4505-9788-8B5EAC201E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{20390CD0-9F3C-4FAF-AAB0-2CABDDBF005D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{20390CD0-9F3C-4FAF-AAB0-2CABDDBF005D}"/>
   </bookViews>
   <sheets>
     <sheet name="Features" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="66">
   <si>
     <t>SMT Refresh Required Features</t>
   </si>
@@ -527,16 +527,10 @@
     <t>Fearure - Firmware Upgrade</t>
   </si>
   <si>
-    <t>UPS should support firmware upgrade for all major MCUs in the system, such as MC, CC, and Adaptor.</t>
-  </si>
-  <si>
     <t>The firmware upgrade image should inlcude all firmware components of the major MCUs in the system.</t>
   </si>
   <si>
     <t>The firmware upgrade image uses an APC proprietary format.</t>
-  </si>
-  <si>
-    <t>The firmware upgrade image should be digitally signed by SE.</t>
   </si>
   <si>
     <t>Adaptor is responsible for receving the firmware upgrade image from external.</t>
@@ -554,9 +548,6 @@
   </si>
   <si>
     <t>Adaptor starts the firmware validation after the whole firmware upgrade image has been received and stored in external serial flash.</t>
-  </si>
-  <si>
-    <t>If the Adaptor validates the firmware upgrade image as valid, Adaptor should start the firmware installation step.</t>
   </si>
   <si>
     <t>If the Adaptor validates the firmware upgrade image as invalid, Adaptor should reject the firmware installation step.</t>
@@ -587,13 +578,37 @@
 * Group Outlets 1</t>
   </si>
   <si>
-    <t>Details</t>
-  </si>
-  <si>
     <t>Fearure - Swithced Outlet Group (SOG)</t>
   </si>
   <si>
     <t>The communication protocol between Adaptor and UPS is switched from the  protocol used under normal conditions to Xmodem with 128 bytes CRC mode.</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>The UPS must support firmware upgrade with output on while input is acceptable for working in bypass mode.</t>
+  </si>
+  <si>
+    <t>The firmware upgrade image must be digitally signed by SE.</t>
+  </si>
+  <si>
+    <t>UPS must support firmware upgrade for all major MCUs in the system, such as MC, CC, and Adaptor.</t>
+  </si>
+  <si>
+    <t>How will we achieve this?</t>
+  </si>
+  <si>
+    <t>UPS LCD must display a message indicating the firmware image transfer is in porgress.</t>
+  </si>
+  <si>
+    <t>If the Adaptor validates the firmware upgrade image as valid and firmware upgrade command is not FWInstall, UPS LCD must display a message indicating a new firmware is availale, but only if the new firmware differs from currently running version.</t>
+  </si>
+  <si>
+    <t>If the Adaptor validates the firmware upgrade image as valid and the firmware upgrade command is FWInstall, Adaptor should start the firmware installation step.</t>
+  </si>
+  <si>
+    <t>LCD must display firmware upgrade completion percentage while the UPS is operating in bootload mode to update  system firmware.</t>
   </si>
 </sst>
 </file>
@@ -740,14 +755,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1085,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB916F49-11FB-4EDF-B993-765135D334E9}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,34 +1303,38 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B0F75-DACA-4E68-87B5-F2FCA539643A}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.85546875" style="12" customWidth="1"/>
     <col min="2" max="2" width="71.7109375" style="12" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="12"/>
+    <col min="3" max="3" width="35.5703125" style="12" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="16"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="18"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C2" s="14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="12">
         <v>1</v>
       </c>
@@ -1323,7 +1342,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>2</v>
       </c>
@@ -1331,7 +1350,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>3</v>
       </c>
@@ -1339,7 +1358,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>4</v>
       </c>
@@ -1347,15 +1366,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>5</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="C7" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>6</v>
       </c>
@@ -1373,34 +1395,34 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CA4D097-EB0E-4CC4-85E1-D8AEFC1F42DF}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="74" style="2" customWidth="1"/>
-    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="3" max="3" width="55.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="19"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>58</v>
+      <c r="C2" s="16" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1408,7 +1430,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1416,42 +1441,48 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>43</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="12">
         <v>3</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>44</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C5" s="13"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="12">
         <v>4</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>45</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="C6" s="13"/>
     </row>
     <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="12">
         <v>5</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="12">
         <v>6</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1459,7 +1490,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1467,7 +1498,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1475,15 +1509,26 @@
         <v>9</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="12">
         <v>10</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>51</v>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="12">
+        <v>10</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1498,8 +1543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC5EE8D-1107-4292-BA48-0DBC134BF805}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1509,20 +1554,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" s="17"/>
-    </row>
-    <row r="2" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="19"/>
+    </row>
+    <row r="2" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>58</v>
+      <c r="C2" s="16" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="135" x14ac:dyDescent="0.25">
@@ -1530,10 +1575,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>53</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -1541,10 +1586,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>54</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1552,7 +1597,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>